<commit_message>
Update Job Application Excel File
</commit_message>
<xml_diff>
--- a/Resume/Job_Applications.xlsx
+++ b/Resume/Job_Applications.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="25600" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Company</t>
   </si>
@@ -34,85 +47,106 @@
     <t>ASML</t>
   </si>
   <si>
+    <t>Algorithm Engineer Intern</t>
+  </si>
+  <si>
+    <t>https://asml.wd3.myworkdayjobs.com/en-US/ASMLEXT1/userHome</t>
+  </si>
+  <si>
+    <t>Develop and improve algorithms for optical metrology; optimization, regression, error prediction</t>
+  </si>
+  <si>
+    <t>Python, MATLAB, C/C++; Optimization, Regression, Bayes rule, Communication skills</t>
+  </si>
+  <si>
     <t>IBM</t>
   </si>
   <si>
+    <t>Researcher Intern - Data for LLMs</t>
+  </si>
+  <si>
+    <t>https://krb-sjobs.brassring.com/TGnewUI/Search/Home/Home?partnerid=26059&amp;siteid=5016#home</t>
+  </si>
+  <si>
+    <t>Define problems, build prototypes, data pipeline development for IBM's Granite models</t>
+  </si>
+  <si>
+    <t>Data Science, NLP, Backend Engineering, Python, Distributed Computing</t>
+  </si>
+  <si>
     <t>eBay</t>
   </si>
   <si>
+    <t>Applied Researcher Intern</t>
+  </si>
+  <si>
+    <t>https://app.ripplematch.com/v2/public/job/e37cac0e/apply?tl=654980d7&amp;from_page=tracking_link</t>
+  </si>
+  <si>
+    <t>Build ML models, data pipelines for e-commerce; conduct experiments, improve models</t>
+  </si>
+  <si>
+    <t>PhD candidate, Python, Java, Scala, Big Data (Hadoop, Spark), SQL, NoSQL (MongoDB)</t>
+  </si>
+  <si>
+    <t>Foundation Models for Data Research Intern</t>
+  </si>
+  <si>
+    <t>https://careers.ibm.com/apply/join/?job=21087648&amp;codes=JB_EPH_Handshake</t>
+  </si>
+  <si>
+    <t>Research for foundation models in data tasks, code generation for SQL, knowledge graphs and multi-modal data</t>
+  </si>
+  <si>
+    <t>LLM, NLP, SQL, Code Generation, Knowledge Graphs, Text-to-SQL, Multi-modal Data</t>
+  </si>
+  <si>
     <t>KLA Corporation</t>
   </si>
   <si>
-    <t>Algorithm Engineer Intern</t>
-  </si>
-  <si>
-    <t>Researcher Intern - Data for LLMs</t>
-  </si>
-  <si>
-    <t>Applied Researcher Intern</t>
-  </si>
-  <si>
-    <t>Foundation Models for Data Research Intern</t>
-  </si>
-  <si>
     <t>Software Engineer (AI/ML) Intern</t>
   </si>
   <si>
-    <t>https://asml.wd3.myworkdayjobs.com/en-US/ASMLEXT1/userHome</t>
-  </si>
-  <si>
-    <t>https://krb-sjobs.brassring.com/TGnewUI/Search/Home/Home?partnerid=26059&amp;siteid=5016#home</t>
-  </si>
-  <si>
-    <t>https://app.ripplematch.com/v2/public/job/e37cac0e/apply?tl=654980d7&amp;from_page=tracking_link</t>
-  </si>
-  <si>
-    <t>https://careers.ibm.com/apply/join/?job=21087648&amp;codes=JB_EPH_Handshake</t>
-  </si>
-  <si>
     <t>https://kla.wd1.myworkdayjobs.com/en-US/Search/job/Austin%2C-TX/Software-Engineer--AI-ML--Intern_2426147/apply/autofillWithResume</t>
   </si>
   <si>
-    <t>Develop and improve algorithms for optical metrology; optimization, regression, error prediction</t>
-  </si>
-  <si>
-    <t>Define problems, build prototypes, data pipeline development for IBM's Granite models</t>
-  </si>
-  <si>
-    <t>Build ML models, data pipelines for e-commerce; conduct experiments, improve models</t>
-  </si>
-  <si>
-    <t>Research for foundation models in data tasks, code generation for SQL, knowledge graphs and multi-modal data</t>
-  </si>
-  <si>
     <t>Develop AI/ML solutions, software system infrastructure, ML model training, data management for KLA products</t>
   </si>
   <si>
-    <t>Python, MATLAB, C/C++; Optimization, Regression, Bayes rule, Communication skills</t>
-  </si>
-  <si>
-    <t>Data Science, NLP, Backend Engineering, Python, Distributed Computing</t>
-  </si>
-  <si>
-    <t>PhD candidate, Python, Java, Scala, Big Data (Hadoop, Spark), SQL, NoSQL (MongoDB)</t>
-  </si>
-  <si>
-    <t>LLM, NLP, SQL, Code Generation, Knowledge Graphs, Text-to-SQL, Multi-modal Data</t>
-  </si>
-  <si>
     <t>Python, C++, C#, Java; Machine Learning, Deep Learning, Distributed Systems, TensorFlow, PyTorch</t>
+  </si>
+  <si>
+    <t>T-Mobile</t>
+  </si>
+  <si>
+    <t>Full Stack Developer Intern</t>
+  </si>
+  <si>
+    <t>https://tmobile.wd1.myworkdayjobs.com/en-US/External/userHome</t>
+  </si>
+  <si>
+    <t>Develop AI-driven full-stack applications, model optimization, data preprocessing, deploy and monitor AI models</t>
+  </si>
+  <si>
+    <t>Machine Learning, Full-Stack Development, Python, Front-end and Back-end Development, Data Analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -120,7 +154,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -128,18 +162,347 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -162,12 +525,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
@@ -175,14 +777,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -465,17 +1118,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="$A7:$XFD7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -499,94 +1154,113 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2" location="home"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://asml.wd3.myworkdayjobs.com/en-US/ASMLEXT1/userHome"/>
+    <hyperlink ref="C3" r:id="rId2" location="home" display="https://krb-sjobs.brassring.com/TGnewUI/Search/Home/Home?partnerid=26059&amp;siteid=5016#home"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://app.ripplematch.com/v2/public/job/e37cac0e/apply?tl=654980d7&amp;from_page=tracking_link"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://careers.ibm.com/apply/join/?job=21087648&amp;codes=JB_EPH_Handshake"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://kla.wd1.myworkdayjobs.com/en-US/Search/job/Austin%2C-TX/Software-Engineer--AI-ML--Intern_2426147/apply/autofillWithResume"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://tmobile.wd1.myworkdayjobs.com/en-US/External/userHome"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Application 10 Jobs 11/11
</commit_message>
<xml_diff>
--- a/Resume/Job_Applications.xlsx
+++ b/Resume/Job_Applications.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Company</t>
   </si>
@@ -129,6 +129,51 @@
   </si>
   <si>
     <t>Machine Learning, Full-Stack Development, Python, Front-end and Back-end Development, Data Analysis</t>
+  </si>
+  <si>
+    <t>Dow Jones</t>
+  </si>
+  <si>
+    <t>Data Analyst Intern</t>
+  </si>
+  <si>
+    <t>https://dowjones.wd1.myworkdayjobs.com/en-US/Dow_Jones_Career/userHome</t>
+  </si>
+  <si>
+    <t>Data reporting, trend analysis, build dashboards, support data pipeline, visualize data insights</t>
+  </si>
+  <si>
+    <t>SQL, Python, Excel (advanced formulas), Tableau/Google Analytics, quantitative analysis, cloud (AWS/S3 a plus)</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Explorer Intern - First-Year Students</t>
+  </si>
+  <si>
+    <t>https://jobs.careers.microsoft.com/global/en/apply/thankyou?Job_id=1782349</t>
+  </si>
+  <si>
+    <t>Hands-on with development tools, collaborate on design and implementation, experience in Software/Product/Program Mgmt</t>
+  </si>
+  <si>
+    <t>Pursuing Bachelor’s in tech field, Intro to CS course, calculus, interest in CS/Software Engineering, teamwork, problem-solving</t>
+  </si>
+  <si>
+    <t>Refonte Learning</t>
+  </si>
+  <si>
+    <t>AI Engineering Training &amp; Internship</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4074161641/?alternateChannel=search&amp;refId=W%2BLRz14TtQDBlwjGM%2FUzdQ%3D%3D&amp;trackingId=G8cGFxuowHCancZVCRKAPg%3D%3D</t>
+  </si>
+  <si>
+    <t>Master AI fundamentals, develop and optimize models, preprocess data, and work on real-world AI projects</t>
+  </si>
+  <si>
+    <t>TensorFlow, Keras, PyTorch, Scikit-learn; model development, data preprocessing, machine learning (ML, DL, CV); cloud (AWS, GCP)</t>
   </si>
 </sst>
 </file>
@@ -165,11 +210,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -626,19 +671,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -648,7 +693,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -772,12 +817,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1124,13 +1177,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="$A7:$XFD7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="14.9090909090909" customWidth="1"/>
+    <col min="4" max="4" width="54.5454545454545" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -1241,7 +1298,7 @@
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
@@ -1250,6 +1307,60 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" ht="29" spans="1:5">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1259,6 +1370,9 @@
     <hyperlink ref="C5" r:id="rId4" display="https://careers.ibm.com/apply/join/?job=21087648&amp;codes=JB_EPH_Handshake"/>
     <hyperlink ref="C6" r:id="rId5" display="https://kla.wd1.myworkdayjobs.com/en-US/Search/job/Austin%2C-TX/Software-Engineer--AI-ML--Intern_2426147/apply/autofillWithResume"/>
     <hyperlink ref="C7" r:id="rId6" display="https://tmobile.wd1.myworkdayjobs.com/en-US/External/userHome"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://jobs.careers.microsoft.com/global/en/apply/thankyou?Job_id=1782349"/>
+    <hyperlink ref="C8" r:id="rId8" display="https://dowjones.wd1.myworkdayjobs.com/en-US/Dow_Jones_Career/userHome"/>
+    <hyperlink ref="C10" r:id="rId9" display="https://www.linkedin.com/jobs/view/4074161641/?alternateChannel=search&amp;refId=W%2BLRz14TtQDBlwjGM%2FUzdQ%3D%3D&amp;trackingId=G8cGFxuowHCancZVCRKAPg%3D%3D"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>